<commit_message>
updated logbook + backlog
</commit_message>
<xml_diff>
--- a/Backlog.xlsx
+++ b/Backlog.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lopes\OneDrive\Desktop\TalesOfTheTavern\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="68" documentId="8_{8C05EBD8-655A-4879-A66C-020870575A58}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{0990A332-9B05-4279-81B4-8BAAC51003B3}"/>
+  <xr:revisionPtr revIDLastSave="69" documentId="8_{8C05EBD8-655A-4879-A66C-020870575A58}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{39E46809-3383-4D9B-A297-21B8B6E3F29A}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20520" windowHeight="9435" xr2:uid="{713CC736-D09F-4D5F-8773-3DAEB56EA070}"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="20520" windowHeight="9435" xr2:uid="{713CC736-D09F-4D5F-8773-3DAEB56EA070}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="23">
   <si>
     <t>En tant que …</t>
   </si>
@@ -98,6 +98,9 @@
   </si>
   <si>
     <t>Permettre a n'importe quelle utilisateur de pouvoir noter une histoire</t>
+  </si>
+  <si>
+    <t>Fait</t>
   </si>
 </sst>
 </file>
@@ -484,7 +487,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -519,7 +522,7 @@
         <v>15</v>
       </c>
       <c r="D2" t="s">
-        <v>2</v>
+        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">

</xml_diff>

<commit_message>
Modified Backlog + technical documentation + logbook + Real pLanning
</commit_message>
<xml_diff>
--- a/Backlog.xlsx
+++ b/Backlog.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20730"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lopes\OneDrive\Desktop\TalesOfTheTavern\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrateur\Desktop\TalesOfTheTavern\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="68" documentId="8_{8C05EBD8-655A-4879-A66C-020870575A58}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{0990A332-9B05-4279-81B4-8BAAC51003B3}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20520" windowHeight="9435" xr2:uid="{713CC736-D09F-4D5F-8773-3DAEB56EA070}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20520" windowHeight="9435"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -30,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="25">
   <si>
     <t>En tant que …</t>
   </si>
@@ -98,12 +97,21 @@
   </si>
   <si>
     <t>Permettre a n'importe quelle utilisateur de pouvoir noter une histoire</t>
+  </si>
+  <si>
+    <t>Fais</t>
+  </si>
+  <si>
+    <t>Resultat obtenue</t>
+  </si>
+  <si>
+    <t>Un nouvel Utilisateur peut créer un compte se deconnecter et se reconnecter par la suite</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -148,9 +156,18 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
+  <dxfs count="6">
     <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
@@ -172,13 +189,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{0C5353E1-2B03-4747-B025-B8965E480420}" name="Tableau1" displayName="Tableau1" ref="A1:D8" totalsRowShown="0">
-  <autoFilter ref="A1:D8" xr:uid="{F87B9293-0234-4347-8CAA-FEDBEF61D44B}"/>
-  <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{9204710F-6F6E-4965-A599-EE93D9CA859C}" name="En tant que …" dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{B2D27856-C9C8-4FC0-BD24-37DEFAF2F762}" name="Je souhaite…" dataDxfId="1"/>
-    <tableColumn id="3" xr3:uid="{D10B8E4B-2393-45B7-B15E-425612A5B1A6}" name="Critère d'acceptation" dataDxfId="0"/>
-    <tableColumn id="4" xr3:uid="{8E08E990-1CB7-4E43-9A36-E81BEA29E952}" name="Statut"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A1:E8" totalsRowShown="0" dataDxfId="1">
+  <autoFilter ref="A1:E8"/>
+  <tableColumns count="5">
+    <tableColumn id="1" name="En tant que …" dataDxfId="5"/>
+    <tableColumn id="2" name="Je souhaite…" dataDxfId="4"/>
+    <tableColumn id="3" name="Critère d'acceptation" dataDxfId="3"/>
+    <tableColumn id="6" name="Resultat obtenue" dataDxfId="0"/>
+    <tableColumn id="4" name="Statut" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -480,21 +498,23 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{53C88BE0-20EA-4492-8018-F3DA07F01980}">
-  <dimension ref="A1:D8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="42.1328125" customWidth="1"/>
-    <col min="3" max="3" width="22.19921875" customWidth="1"/>
+    <col min="1" max="1" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="47.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.5703125" customWidth="1"/>
+    <col min="5" max="5" width="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -504,11 +524,14 @@
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="57" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>10</v>
       </c>
@@ -518,11 +541,14 @@
       <c r="C2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+      <c r="D2" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>5</v>
       </c>
@@ -532,11 +558,12 @@
       <c r="C3" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="3"/>
+      <c r="E3" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:5" ht="105" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>9</v>
       </c>
@@ -546,63 +573,68 @@
       <c r="C4" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="3"/>
+      <c r="E4" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="3"/>
+      <c r="E5" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C6" s="1" t="s">
+      <c r="C6" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="D6" t="s">
+      <c r="D6" s="3"/>
+      <c r="E6" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="C7" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D7" s="3"/>
+      <c r="E7" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="42.75" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="1" t="s">
+      <c r="C8" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D8" s="3"/>
+      <c r="E8" s="2" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added the my profile page
</commit_message>
<xml_diff>
--- a/Backlog.xlsx
+++ b/Backlog.xlsx
@@ -37,21 +37,12 @@
     <t>Critère d'acceptation</t>
   </si>
   <si>
-    <t>A faire</t>
-  </si>
-  <si>
     <t>créer un nouveau compte et pourvoir m'y connecter</t>
   </si>
   <si>
-    <t>avoir accès a ma page de gestion d'histoire</t>
-  </si>
-  <si>
     <t>Admin/Membre</t>
   </si>
   <si>
-    <t>que lorsque j'évalue un histoire sa note et la note de l'auteur change</t>
-  </si>
-  <si>
     <t>Je souhaite…</t>
   </si>
   <si>
@@ -64,48 +55,55 @@
     <t>Anonyme</t>
   </si>
   <si>
-    <t>Avoir 2 tri sur la page accueil 1-moyenne de notes (tri croissant) 2-Les histoires plus récentes (tri
-décroissant)</t>
-  </si>
-  <si>
-    <t>avoir mes histoire que j'ai marqué en favoris sur la page accueille et pouvoir les supprimer</t>
-  </si>
-  <si>
-    <t>pouvoir chercher une histoire par son titre ou par son autheur</t>
-  </si>
-  <si>
-    <t>pouvoir évaluer une histoire Selon le style, l'histoire, orthographe et l'originalité.</t>
-  </si>
-  <si>
-    <t>Avoir une page "création de compte" fonctionel et une page de "login" qui permet de se connecter</t>
-  </si>
-  <si>
-    <t>Avoir une page "mon compte" qui affiche les information du compte ( du nom d'utilisateur au histoir qu'il a créer).</t>
-  </si>
-  <si>
-    <t>Pouvoir afficher les hitoire sur la page d'aceuil avec 2 tri différent. 1-moyenne de notes (tri croissant) 2-Les histoires plus récentes (tri
-décroissant)</t>
-  </si>
-  <si>
-    <t>Que les moyenne des histoire / autheur change dans le temps</t>
-  </si>
-  <si>
-    <t>Permettre au utilisateur de chercher une histoir avec le titre</t>
-  </si>
-  <si>
-    <t>afficher sur la page principale des utilisateurs identifier leur histoire favorite et pouvoir les suprimmer</t>
-  </si>
-  <si>
-    <t>Permettre a n'importe quelle utilisateur de pouvoir noter une histoire</t>
-  </si>
-  <si>
     <t>Fais</t>
   </si>
   <si>
     <t>Resultat obtenue</t>
   </si>
   <si>
-    <t>Un nouvel Utilisateur peut créer un compte se deconnecter et se reconnecter par la suite</t>
+    <t>Avoir une page "création du compte" fonctionnel et une page de "login" qui permettent de se connecter</t>
+  </si>
+  <si>
+    <t>Un nouvel utilisateur peut créer un compte se déconnecter et se reconnecter par la suite</t>
+  </si>
+  <si>
+    <t>avoir accès à ma page de gestion d'histoire</t>
+  </si>
+  <si>
+    <t>Avoir une page "mon compte" qui affiche les informations du compte ( du nom d'utilisateur aux histoires qu'il a créé).</t>
+  </si>
+  <si>
+    <t>À faire</t>
+  </si>
+  <si>
+    <t>Avoir 2 tris sur la page accueille 1-moyenne de notes (tri croissant) 2-Les histoires plus récentes (tri décroissant)</t>
+  </si>
+  <si>
+    <t>Pouvoir afficher les histoires sur la page d'accueil avec 2 tris différents. 1-moyenne de notes (tri croissant) 2-Les histoires plus récentes (tri décroissant)</t>
+  </si>
+  <si>
+    <t>avoir mes histoires que j'ai marquées en favoris sur la page accueille et pouvoir les supprimer</t>
+  </si>
+  <si>
+    <t>afficher sur la page principale des utilisateurs identifier leur histoire favorite et pouvoir les supprimer</t>
+  </si>
+  <si>
+    <t>pouvoir évaluer une histoire selon le style, l'histoire, orthographe et l'originalité.</t>
+  </si>
+  <si>
+    <t>Permettre à n'importe quel utilisateur de pouvoir noter une histoire</t>
+  </si>
+  <si>
+    <t>que lorsque j'évalue une histoire sa note et la note de l'auteur change</t>
+  </si>
+  <si>
+    <t>Que les moyenne des histoire / auteur change dans le temps</t>
+  </si>
+  <si>
+    <t>pouvoir chercher une histoire par son titre ou par son auteur</t>
+  </si>
+  <si>
+    <t>Permettre aux utilisateurs de chercher une histoire avec le titre</t>
   </si>
 </sst>
 </file>
@@ -158,12 +156,6 @@
   </cellStyles>
   <dxfs count="6">
     <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -173,7 +165,13 @@
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -189,14 +187,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A1:E8" totalsRowShown="0" dataDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A1:E8" totalsRowShown="0" dataDxfId="5">
   <autoFilter ref="A1:E8"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="En tant que …" dataDxfId="5"/>
-    <tableColumn id="2" name="Je souhaite…" dataDxfId="4"/>
-    <tableColumn id="3" name="Critère d'acceptation" dataDxfId="3"/>
-    <tableColumn id="6" name="Resultat obtenue" dataDxfId="0"/>
-    <tableColumn id="4" name="Statut" dataDxfId="2"/>
+    <tableColumn id="1" name="En tant que …" dataDxfId="4"/>
+    <tableColumn id="2" name="Je souhaite…" dataDxfId="3"/>
+    <tableColumn id="3" name="Critère d'acceptation" dataDxfId="2"/>
+    <tableColumn id="6" name="Resultat obtenue" dataDxfId="1"/>
+    <tableColumn id="4" name="Statut" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -502,7 +500,7 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -519,123 +517,123 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>23</v>
+        <v>9</v>
       </c>
       <c r="E1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" s="2" t="s">
         <v>8</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="60" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="D3" s="3"/>
       <c r="E3" s="2" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="105" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>11</v>
+        <v>15</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D4" s="3"/>
       <c r="E4" s="2" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D5" s="3"/>
       <c r="E5" s="2" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D6" s="3"/>
       <c r="E6" s="2" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="D7" s="3"/>
       <c r="E7" s="2" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>13</v>
+        <v>23</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="D8" s="3"/>
       <c r="E8" s="2" t="s">
-        <v>2</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modified backlog + documentaion + logbook
</commit_message>
<xml_diff>
--- a/Backlog.xlsx
+++ b/Backlog.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -15,14 +15,10 @@
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -500,7 +496,7 @@
   <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -558,7 +554,7 @@
       </c>
       <c r="D3" s="3"/>
       <c r="E3" s="2" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
     </row>
     <row r="4" spans="1:5" ht="105" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Modified backlog + documentation + logbook
</commit_message>
<xml_diff>
--- a/Backlog.xlsx
+++ b/Backlog.xlsx
@@ -15,7 +15,6 @@
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,14 +24,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="36">
   <si>
     <t>En tant que …</t>
   </si>
   <si>
-    <t>Critère d'acceptation</t>
-  </si>
-  <si>
     <t>créer un nouveau compte et pourvoir m'y connecter</t>
   </si>
   <si>
@@ -100,13 +96,49 @@
   </si>
   <si>
     <t>Permettre aux utilisateurs de chercher une histoire avec le titre</t>
+  </si>
+  <si>
+    <t>fais</t>
+  </si>
+  <si>
+    <t>La page de gestion d'histoire s'affiche</t>
+  </si>
+  <si>
+    <t>Pour</t>
+  </si>
+  <si>
+    <t>User Stories</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>A14</t>
+  </si>
+  <si>
+    <t>A15</t>
+  </si>
+  <si>
+    <t>A16</t>
+  </si>
+  <si>
+    <t>A17</t>
+  </si>
+  <si>
+    <t>A18</t>
+  </si>
+  <si>
+    <t>A19</t>
+  </si>
+  <si>
+    <t>A20</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -114,13 +146,26 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -135,7 +180,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -145,6 +190,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -183,12 +231,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A1:E8" totalsRowShown="0" dataDxfId="5">
-  <autoFilter ref="A1:E8"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="B2:F9" totalsRowShown="0" dataDxfId="5">
+  <autoFilter ref="B2:F9"/>
   <tableColumns count="5">
     <tableColumn id="1" name="En tant que …" dataDxfId="4"/>
     <tableColumn id="2" name="Je souhaite…" dataDxfId="3"/>
-    <tableColumn id="3" name="Critère d'acceptation" dataDxfId="2"/>
+    <tableColumn id="3" name="Pour" dataDxfId="2"/>
     <tableColumn id="6" name="Resultat obtenue" dataDxfId="1"/>
     <tableColumn id="4" name="Statut" dataDxfId="0"/>
   </tableColumns>
@@ -493,149 +541,190 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="22.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="47.7109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="24.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.5703125" customWidth="1"/>
-    <col min="5" max="5" width="9" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="47.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.5703125" customWidth="1"/>
+    <col min="6" max="6" width="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="1" t="s">
+    </row>
+    <row r="3" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>29</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D3" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
+      <c r="C5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="3"/>
+      <c r="F5" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="2" t="s">
+    </row>
+    <row r="6" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>32</v>
+      </c>
+      <c r="B6" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="A3" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="3" t="s">
+      <c r="C6" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E6" s="3"/>
+      <c r="F6" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E7" s="3"/>
+      <c r="F7" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="3"/>
-      <c r="E3" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" ht="105" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" s="3"/>
-      <c r="E4" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="75" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D5" s="3"/>
-      <c r="E5" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C6" s="3" t="s">
+    </row>
+    <row r="8" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>34</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="D6" s="3"/>
-      <c r="E6" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="3" t="s">
+      <c r="D8" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="E8" s="3"/>
+      <c r="F8" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="D7" s="3"/>
-      <c r="E7" s="2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="45" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="3" t="s">
+      <c r="D9" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="C8" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="D8" s="3"/>
-      <c r="E8" s="2" t="s">
-        <v>14</v>
+      <c r="E9" s="3"/>
+      <c r="F9" s="2" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:F1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>